<commit_message>
rough analysis done up to and including neural nets
</commit_message>
<xml_diff>
--- a/Assignment1/Analysis/analysis.xlsx
+++ b/Assignment1/Analysis/analysis.xlsx
@@ -221,11 +221,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -927,11 +927,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127007000"/>
-        <c:axId val="2127015832"/>
+        <c:axId val="-2145965400"/>
+        <c:axId val="-2145956520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127007000"/>
+        <c:axId val="-2145965400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,7 +965,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127015832"/>
+        <c:crossAx val="-2145956520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -975,7 +975,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127015832"/>
+        <c:axId val="-2145956520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -1007,7 +1007,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127007000"/>
+        <c:crossAx val="-2145965400"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1624,11 +1624,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126751160"/>
-        <c:axId val="2126743480"/>
+        <c:axId val="-2146562296"/>
+        <c:axId val="-2146554600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126751160"/>
+        <c:axId val="-2146562296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1662,7 +1662,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126743480"/>
+        <c:crossAx val="-2146554600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1672,7 +1672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126743480"/>
+        <c:axId val="-2146554600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1704,7 +1704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126751160"/>
+        <c:crossAx val="-2146562296"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2321,11 +2321,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127109368"/>
-        <c:axId val="2127116840"/>
+        <c:axId val="-2145844744"/>
+        <c:axId val="-2145837272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127109368"/>
+        <c:axId val="-2145844744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2359,7 +2359,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127116840"/>
+        <c:crossAx val="-2145837272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2369,7 +2369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127116840"/>
+        <c:axId val="-2145837272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2401,7 +2401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127109368"/>
+        <c:crossAx val="-2145844744"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3022,11 +3022,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127176504"/>
-        <c:axId val="2127184232"/>
+        <c:axId val="-2145777608"/>
+        <c:axId val="-2145769880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127176504"/>
+        <c:axId val="-2145777608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3060,7 +3060,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127184232"/>
+        <c:crossAx val="-2145769880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3070,7 +3070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127184232"/>
+        <c:axId val="-2145769880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -3102,7 +3102,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127176504"/>
+        <c:crossAx val="-2145777608"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3719,11 +3719,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127244968"/>
-        <c:axId val="2127252696"/>
+        <c:axId val="-2146971288"/>
+        <c:axId val="-2146963560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127244968"/>
+        <c:axId val="-2146971288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3757,7 +3757,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127252696"/>
+        <c:crossAx val="-2146963560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3767,11 +3767,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127252696"/>
+        <c:axId val="-2146963560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
-          <c:min val="0.87"/>
+          <c:min val="0.79"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3799,7 +3799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127244968"/>
+        <c:crossAx val="-2146971288"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4420,11 +4420,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127311400"/>
-        <c:axId val="2127319128"/>
+        <c:axId val="-2146902360"/>
+        <c:axId val="-2146894632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127311400"/>
+        <c:axId val="-2146902360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4458,7 +4458,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127319128"/>
+        <c:crossAx val="-2146894632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4468,7 +4468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127319128"/>
+        <c:axId val="-2146894632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.75"/>
@@ -4500,7 +4500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127311400"/>
+        <c:crossAx val="-2146902360"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5117,11 +5117,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127379288"/>
-        <c:axId val="2127387016"/>
+        <c:axId val="-2146833928"/>
+        <c:axId val="-2146826200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127379288"/>
+        <c:axId val="-2146833928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5155,7 +5155,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127387016"/>
+        <c:crossAx val="-2146826200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5165,7 +5165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127387016"/>
+        <c:axId val="-2146826200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -5197,7 +5197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127379288"/>
+        <c:crossAx val="-2146833928"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5818,11 +5818,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127447320"/>
-        <c:axId val="2127455080"/>
+        <c:axId val="-2146765896"/>
+        <c:axId val="-2146758136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127447320"/>
+        <c:axId val="-2146765896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5856,7 +5856,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127455080"/>
+        <c:crossAx val="-2146758136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5866,7 +5866,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127455080"/>
+        <c:axId val="-2146758136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.85"/>
@@ -5898,7 +5898,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127447320"/>
+        <c:crossAx val="-2146765896"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6515,11 +6515,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127515192"/>
-        <c:axId val="2127522952"/>
+        <c:axId val="-2146698024"/>
+        <c:axId val="-2146690264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127515192"/>
+        <c:axId val="-2146698024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6553,7 +6553,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127522952"/>
+        <c:crossAx val="-2146690264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6563,7 +6563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127522952"/>
+        <c:axId val="-2146690264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9996"/>
@@ -6595,7 +6595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127515192"/>
+        <c:crossAx val="-2146698024"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7216,11 +7216,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126819960"/>
-        <c:axId val="2126812280"/>
+        <c:axId val="-2146631288"/>
+        <c:axId val="-2146623528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126819960"/>
+        <c:axId val="-2146631288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7254,7 +7254,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126812280"/>
+        <c:crossAx val="-2146623528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7264,7 +7264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126812280"/>
+        <c:axId val="-2146623528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -7296,7 +7296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126819960"/>
+        <c:crossAx val="-2146631288"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7968,2135 +7968,2135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="14.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>0.2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.78273809523809501</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.80572289156626498</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>0.2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0.99861256135469401</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>0.99877579751690904</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1">
         <v>0.1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.84375</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.82379518072289104</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>0.1</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>0.88186333541211104</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>0.88251226752904899</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
         <v>0.2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.84375</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.82379518072289104</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
         <v>0.2</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>0.88186333541211104</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>0.88251226752904899</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1">
         <v>0.4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.58957999999999999</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.51204819277108404</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
         <v>0.4</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>0.79192426344536904</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>0.79259459514603703</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>0.4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.78614457831325302</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.79919678714859399</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>0.4</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>0.99890841143756004</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>0.99904104464923305</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
         <v>0.1</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>0.83734939759036098</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>0.81726907630522005</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
         <v>0.1</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>0.88204689020037497</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>0.88260618220151599</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
         <v>0.2</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.843373493975903</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>0.81726907630522005</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
         <v>0.2</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>0.88204689020037497</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>0.88260618220151599</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
         <v>0.4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.58433734939758997</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.47188755020080297</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
         <v>0.4</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>0.79299545036696195</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>0.792103920835175</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>0.6</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0.80718699186991805</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>0.82831325301204795</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>0.6</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>0.99907504497699595</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>0.99908184813768197</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1">
         <v>0.1</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>0.84331707317073101</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>0.80421686746987897</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
         <v>0.1</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>0.88220413486118399</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>0.88264999030839697</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1">
         <v>0.2</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.84331707317073101</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>0.80421686746987897</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
         <v>0.2</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>0.88220413486118399</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>0.88264999030839697</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
         <v>0.4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>0.50401626016260104</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>0.53012048192771</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
         <v>0.4</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>0.79321109419542002</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>0.79133468675718899</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>0.8</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.81330067138450302</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.77710843373493899</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>0.8</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>0.99913795174578601</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>0.99926548600342702</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1">
         <v>0.1</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>0.84336780983487503</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>0.76506024096385505</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
         <v>0.1</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>0.88255248596134495</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>0.88170244021872102</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1">
         <v>0.2</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>0.84336780983487503</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>0.76506024096385505</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
         <v>0.2</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>0.88255248596134495</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>0.88170244021872102</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1">
         <v>0.4</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>0.51506078751587703</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>0.51204819277108404</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1">
         <v>0.4</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>0.79280777379621603</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>0.79107157430833197</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="F20" s="1" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="F20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>0.2</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>0.18</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>0.84375</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>0.82379518072289104</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>0.2</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>0.18</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="1">
         <v>0.894574806309402</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="1">
         <v>0.89642226824316695</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1">
         <v>0.36</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>0.75624999999999998</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>0.82379518072289104</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
         <v>0.36</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <v>0.87965961357077904</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <v>0.88251226752904899</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1">
         <v>0.54</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>0.52410714285714199</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>0.51204819277108404</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
         <v>0.54</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>0.79192426344536904</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <v>0.79259459514603703</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1">
         <v>0.72</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>0.52410714285714199</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>0.51204819277108404</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
         <v>0.72</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>0.79192426344536904</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>0.79259459514603703</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>0.4</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>0.18</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>0.843373493975903</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>0.81726907630522005</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>0.4</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>0.18</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
         <v>0.89623760146262199</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="1">
         <v>0.89609956813003699</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1">
         <v>0.36</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>0.843373493975903</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>0.81726907630522005</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
         <v>0.36</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
         <v>0.87703791280708399</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="1">
         <v>0.87619274322440199</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1">
         <v>0.54</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>0.50602409638554202</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>0.47188755020080297</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
         <v>0.54</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>0.79299545036696195</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="1">
         <v>0.792103920835175</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1">
         <v>0.72</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>0.50602409638554202</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>0.47188755020080297</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
         <v>0.72</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>0.79299545036696195</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="1">
         <v>0.792103920835175</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>0.6</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>0.18</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>0.84331707317073101</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>0.80421686746987897</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>0.6</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>0.18</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>0.89639133392294201</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="1">
         <v>0.89579996531426298</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1">
         <v>0.36</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>0.84331707317073101</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>0.80421686746987897</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
         <v>0.36</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="1">
         <v>0.87586547340097698</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="1">
         <v>0.87616171714801605</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1">
         <v>0.54</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>0.50401626016260104</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>0.53012048192771</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
         <v>0.54</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>0.79321109419542002</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <v>0.79133468675718899</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1">
         <v>0.72</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>0.50401626016260104</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>0.53012048192771</v>
       </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1">
         <v>0.72</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="1">
         <v>0.79321109419542002</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="1">
         <v>0.79133468675718899</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>0.8</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>0.18</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>0.84336780983487503</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>0.76506024096385505</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>0.8</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <v>0.18</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="1">
         <v>0.89636053157413897</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="1">
         <v>0.89533175548845101</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1">
         <v>0.36</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>0.84336780983487503</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>0.76506024096385505</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1">
         <v>0.36</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="1">
         <v>0.87618660005567195</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="1">
         <v>0.87517342691585698</v>
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1">
         <v>0.54</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>0.51506078751587703</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>0.51204819277108404</v>
       </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1">
         <v>0.54</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="1">
         <v>0.79280777379621603</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="1">
         <v>0.79107157430833197</v>
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1">
         <v>0.72</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>0.51506078751587703</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="1">
         <v>0.51204819277108404</v>
       </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1">
         <v>0.72</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="1">
         <v>0.79280777379621603</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="1">
         <v>0.79107157430833197</v>
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="F39" s="1" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="F39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>0.2</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>1</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>0.43958333333333299</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>0.41415662650602397</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>0.2</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>1</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="1">
         <v>0.98518699294267698</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="1">
         <v>0.982810156799934</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1">
         <v>5</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>0.45148809523809502</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>0.421686746987951</v>
       </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2">
+      <c r="F42" s="1"/>
+      <c r="G42" s="1">
         <v>5</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="1">
         <v>0.98728857905578304</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="1">
         <v>0.98726829417585604</v>
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1">
         <v>10</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>0.48809523809523803</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>0.47590361445783103</v>
       </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2">
+      <c r="F43" s="1"/>
+      <c r="G43" s="1">
         <v>10</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="1">
         <v>0.99045117978993003</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="1">
         <v>0.99004825398120799</v>
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1">
         <v>15</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>0.50624999999999998</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <v>0.483433734939759</v>
       </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2">
+      <c r="F44" s="1"/>
+      <c r="G44" s="1">
         <v>15</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="1">
         <v>0.99075723728107301</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="1">
         <v>0.99108372524815602</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>0.4</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>1</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>0.36144578313253001</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="1">
         <v>0.369477911646586</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="1">
         <v>0.4</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
         <v>1</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="1">
         <v>0.98371793751949499</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="1">
         <v>0.98506478049444002</v>
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1">
         <v>5</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>0.50301204819277101</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <v>0.41365461847389501</v>
       </c>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1">
         <v>5</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="1">
         <v>0.99008384289292595</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="1">
         <v>0.99074370047947702</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1">
         <v>10</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>0.50301204819277101</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="1">
         <v>0.47188755020080297</v>
       </c>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2">
+      <c r="F47" s="1"/>
+      <c r="G47" s="1">
         <v>10</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="1">
         <v>0.99373608797797397</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="1">
         <v>0.995817322406229</v>
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1">
         <v>15</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>0.50301204819277101</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <v>0.47188755020080297</v>
       </c>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2">
+      <c r="F48" s="1"/>
+      <c r="G48" s="1">
         <v>15</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="1">
         <v>0.99615391234282702</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="1">
         <v>0.996946305301458</v>
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>0.6</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>1</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>0.385398373983739</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="1">
         <v>0.38855421686746899</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="1">
         <v>0.6</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="1">
         <v>1</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="1">
         <v>0.98526191599545798</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="1">
         <v>0.98594207481917495</v>
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1">
         <v>5</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>0.37123577235772298</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="1">
         <v>0.469879518072289</v>
       </c>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2">
+      <c r="F50" s="1"/>
+      <c r="G50" s="1">
         <v>5</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="1">
         <v>0.99089326287021096</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I50" s="1">
         <v>0.99548065249992301</v>
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1">
         <v>10</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>0.49398373983739802</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="1">
         <v>0.469879518072289</v>
       </c>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2">
+      <c r="F51" s="1"/>
+      <c r="G51" s="1">
         <v>10</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="1">
         <v>0.99662663131343798</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="1">
         <v>0.99661303979678195</v>
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1">
         <v>15</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>0.51014634146341398</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="1">
         <v>0.63253012048192703</v>
       </c>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2">
+      <c r="F52" s="1"/>
+      <c r="G52" s="1">
         <v>15</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="1">
         <v>0.99685787719235996</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I52" s="1">
         <v>0.99707211572794097</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>0.8</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>1</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>0.40043549265106099</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="1">
         <v>0.42771084337349302</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="1">
         <v>0.8</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="1">
         <v>1</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="1">
         <v>0.98605931777669797</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I53" s="1">
         <v>0.98683995756141296</v>
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1">
         <v>5</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>0.38687171112320801</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="1">
         <v>0.41566265060240898</v>
       </c>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2">
+      <c r="F54" s="1"/>
+      <c r="G54" s="1">
         <v>5</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="1">
         <v>0.99433291380685795</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I54" s="1">
         <v>0.996531461682853</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1">
         <v>10</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>0.55562511340954401</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="1">
         <v>0.60240963855421603</v>
       </c>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2">
+      <c r="F55" s="1"/>
+      <c r="G55" s="1">
         <v>10</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="1">
         <v>0.99674054345525998</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="1">
         <v>0.99706194401371095</v>
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1">
         <v>15</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>0.692741789148974</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="1">
         <v>0.70481927710843295</v>
       </c>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2">
+      <c r="F56" s="1"/>
+      <c r="G56" s="1">
         <v>15</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56" s="1">
         <v>0.99702109043010301</v>
       </c>
-      <c r="I56" s="2">
+      <c r="I56" s="1">
         <v>0.99755162001142506</v>
       </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="F58" s="1" t="s">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="F58" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="I59" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>0.2</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>1</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>0.66279761904761902</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="1">
         <v>0.75451807228915602</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="1">
         <v>0.2</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="1">
         <v>1</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H60" s="1">
         <v>0.99951030901383497</v>
       </c>
-      <c r="I60" s="2">
+      <c r="I60" s="1">
         <v>0.99944400803892897</v>
       </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1">
         <v>2</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>0.73452380952380902</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="1">
         <v>0.76054216867469804</v>
       </c>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2">
+      <c r="F61" s="1"/>
+      <c r="G61" s="1">
         <v>2</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61" s="1">
         <v>0.99932667218768401</v>
       </c>
-      <c r="I61" s="2">
+      <c r="I61" s="1">
         <v>0.99923997429174705</v>
       </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1">
         <v>3</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>0.74732142857142803</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="1">
         <v>0.82379518072289104</v>
       </c>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1">
         <v>3</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62" s="1">
         <v>0.99940828485424205</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I62" s="1">
         <v>0.99930118441590199</v>
       </c>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1">
         <v>4</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>0.72916666666666596</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="1">
         <v>0.78915662650602403</v>
       </c>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2">
+      <c r="F63" s="1"/>
+      <c r="G63" s="1">
         <v>4</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63" s="1">
         <v>0.99902061303179202</v>
       </c>
-      <c r="I63" s="2">
+      <c r="I63" s="1">
         <v>0.99911755404343805</v>
       </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="2">
+      <c r="A64" s="1">
         <v>0.4</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>1</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <v>0.75602409638554202</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="1">
         <v>0.708835341365461</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="1">
         <v>0.4</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="1">
         <v>1</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64" s="1">
         <v>0.99945930609410005</v>
       </c>
-      <c r="I64" s="2">
+      <c r="I64" s="1">
         <v>0.99942870745060697</v>
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1">
         <v>2</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="1">
         <v>0.73795180722891496</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="1">
         <v>0.72489959839357399</v>
       </c>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2">
+      <c r="F65" s="1"/>
+      <c r="G65" s="1">
         <v>2</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="1">
         <v>0.99939809409644598</v>
       </c>
-      <c r="I65" s="2">
+      <c r="I65" s="1">
         <v>0.99936749753459997</v>
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1">
         <v>3</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="1">
         <v>0.80421686746987897</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="1">
         <v>0.78714859437750995</v>
       </c>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2">
+      <c r="F66" s="1"/>
+      <c r="G66" s="1">
         <v>3</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="1">
         <v>0.99944910118022801</v>
       </c>
-      <c r="I66" s="2">
+      <c r="I66" s="1">
         <v>0.99941510524705002</v>
       </c>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1">
         <v>4</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="1">
         <v>0.80722891566264998</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="1">
         <v>0.82128514056224899</v>
       </c>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2">
+      <c r="F67" s="1"/>
+      <c r="G67" s="1">
         <v>4</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67" s="1">
         <v>0.99931647976486804</v>
       </c>
-      <c r="I67" s="2">
+      <c r="I67" s="1">
         <v>0.99931988982215103</v>
       </c>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="2">
+      <c r="A68" s="1">
         <v>0.6</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>1</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="1">
         <v>0.76305691056910496</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="1">
         <v>0.76807228915662595</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="1">
         <v>0.6</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68" s="1">
         <v>1</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68" s="1">
         <v>0.99943550295521599</v>
       </c>
-      <c r="I68" s="2">
+      <c r="I68" s="1">
         <v>0.99951031900676302</v>
       </c>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1">
         <v>2</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="1">
         <v>0.74079674796747896</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="1">
         <v>0.77409638554216798</v>
       </c>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2">
+      <c r="F69" s="1"/>
+      <c r="G69" s="1">
         <v>2</v>
       </c>
-      <c r="H69" s="2">
+      <c r="H69" s="1">
         <v>0.99946950878791296</v>
       </c>
-      <c r="I69" s="2">
+      <c r="I69" s="1">
         <v>0.99938789875845402</v>
       </c>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1">
         <v>3</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="1">
         <v>0.81731707317073099</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="1">
         <v>0.813253012048192</v>
       </c>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2">
+      <c r="F70" s="1"/>
+      <c r="G70" s="1">
         <v>3</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H70" s="1">
         <v>0.99949671375009796</v>
       </c>
-      <c r="I70" s="2">
+      <c r="I70" s="1">
         <v>0.99946951225732705</v>
       </c>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1">
         <v>4</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="1">
         <v>0.81131707317073098</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="1">
         <v>0.80722891566264998</v>
       </c>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2">
+      <c r="F71" s="1"/>
+      <c r="G71" s="1">
         <v>4</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71" s="1">
         <v>0.99944910580634405</v>
       </c>
-      <c r="I71" s="2">
+      <c r="I71" s="1">
         <v>0.99933689032165895</v>
       </c>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="2">
+      <c r="A72" s="1">
         <v>0.8</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>1</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="1">
         <v>0.76364543639992699</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="1">
         <v>0.77710843373493899</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="1">
         <v>0.8</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="1">
         <v>1</v>
       </c>
-      <c r="H72" s="2">
+      <c r="H72" s="1">
         <v>0.999489912613719</v>
       </c>
-      <c r="I72" s="2">
+      <c r="I72" s="1">
         <v>0.99951032400228501</v>
       </c>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1">
         <v>2</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="1">
         <v>0.77260932680094296</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="1">
         <v>0.75301204819277101</v>
       </c>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2">
+      <c r="F73" s="1"/>
+      <c r="G73" s="1">
         <v>2</v>
       </c>
-      <c r="H73" s="2">
+      <c r="H73" s="1">
         <v>0.99947970998966795</v>
       </c>
-      <c r="I73" s="2">
+      <c r="I73" s="1">
         <v>0.99955113033542797</v>
       </c>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1">
         <v>3</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="1">
         <v>0.81193068408637203</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="1">
         <v>0.75301204819277101</v>
       </c>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2">
+      <c r="F74" s="1"/>
+      <c r="G74" s="1">
         <v>3</v>
       </c>
-      <c r="H74" s="2">
+      <c r="H74" s="1">
         <v>0.99954092094644498</v>
       </c>
-      <c r="I74" s="2">
+      <c r="I74" s="1">
         <v>0.99959193666857005</v>
       </c>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1">
         <v>4</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="1">
         <v>0.81036109598983797</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="1">
         <v>0.73493975903614395</v>
       </c>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2">
+      <c r="F75" s="1"/>
+      <c r="G75" s="1">
         <v>4</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75" s="1">
         <v>0.99943890334429697</v>
       </c>
-      <c r="I75" s="2">
+      <c r="I75" s="1">
         <v>0.99944911450257001</v>
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="G77" s="1" t="s">
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="G77" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="J78" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="K78" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="2">
+      <c r="A79" s="1">
         <v>0.2</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>1</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79" s="1">
         <v>0.52351190476190401</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79" s="1">
         <v>0.53313253012048101</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G79" s="1">
         <v>0.2</v>
       </c>
-      <c r="H79" s="2">
+      <c r="H79" s="1">
         <v>1</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I79" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J79" s="2">
+      <c r="J79" s="1">
         <v>0.45938989825114901</v>
       </c>
-      <c r="K79" s="2">
+      <c r="K79" s="1">
         <v>0.49355763443273498</v>
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2" t="s">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="1">
         <v>0.52351190476190401</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80" s="1">
         <v>0.53313253012048101</v>
       </c>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2" t="s">
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J80" s="2">
+      <c r="J80" s="1">
         <v>0.445960964538549</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K80" s="1">
         <v>0.55493098558501497</v>
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1">
         <v>100</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="1">
         <v>0.753571428571428</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81" s="1">
         <v>0.81777108433734902</v>
       </c>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2">
+      <c r="G81" s="1"/>
+      <c r="H81" s="1">
         <v>100</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="I81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J81" s="2">
+      <c r="J81" s="1">
         <v>0.81822506417044605</v>
       </c>
-      <c r="K81" s="2">
+      <c r="K81" s="1">
         <v>0.84184324087203999</v>
       </c>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2" t="s">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82" s="1">
         <v>0.48005952380952299</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="1">
         <v>0.73343373493975905</v>
       </c>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2" t="s">
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J82" s="2">
+      <c r="J82" s="1">
         <v>0.67067132570613197</v>
       </c>
-      <c r="K82" s="2">
+      <c r="K82" s="1">
         <v>0.18086571518929201</v>
       </c>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83" s="2">
+      <c r="A83" s="1">
         <v>0.4</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>1</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83" s="1">
         <v>0.64759036144578297</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83" s="1">
         <v>0.63855421686746905</v>
       </c>
-      <c r="G83" s="2">
+      <c r="G83" s="1">
         <v>0.4</v>
       </c>
-      <c r="H83" s="2">
+      <c r="H83" s="1">
         <v>1</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I83" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J83" s="2">
+      <c r="J83" s="1">
         <v>0.43002235102617598</v>
       </c>
-      <c r="K83" s="2">
+      <c r="K83" s="1">
         <v>0.48693848403441298</v>
       </c>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2" t="s">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84" s="1">
         <v>0.60843373493975905</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="1">
         <v>0.60441767068273</v>
       </c>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2" t="s">
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J84" s="2">
+      <c r="J84" s="1">
         <v>0.38307852739176002</v>
       </c>
-      <c r="K84" s="2">
+      <c r="K84" s="1">
         <v>0.359764681878464</v>
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1">
         <v>100</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85" s="1">
         <v>0.79819277108433695</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85" s="1">
         <v>0.59036144578313199</v>
       </c>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2">
+      <c r="G85" s="1"/>
+      <c r="H85" s="1">
         <v>100</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I85" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J85" s="2">
+      <c r="J85" s="1">
         <v>0.52866364384728004</v>
       </c>
-      <c r="K85" s="2">
+      <c r="K85" s="1">
         <v>0.50434930458734295</v>
       </c>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2" t="s">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="1">
         <v>0.69277108433734902</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86" s="1">
         <v>0.74297188755020005</v>
       </c>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2" t="s">
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J86" s="2">
+      <c r="J86" s="1">
         <v>0.53029288299314803</v>
       </c>
-      <c r="K86" s="2">
+      <c r="K86" s="1">
         <v>0.89931648927126195</v>
       </c>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="2">
+      <c r="A87" s="1">
         <v>0.6</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>1</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87" s="1">
         <v>0.531983739837398</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87" s="1">
         <v>0.469879518072289</v>
       </c>
-      <c r="G87" s="2">
+      <c r="G87" s="1">
         <v>0.6</v>
       </c>
-      <c r="H87" s="2">
+      <c r="H87" s="1">
         <v>1</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="I87" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J87" s="2">
+      <c r="J87" s="1">
         <v>0.74262640619903697</v>
       </c>
-      <c r="K87" s="2">
+      <c r="K87" s="1">
         <v>0.81096273323607704</v>
       </c>
     </row>
     <row r="88" spans="1:11">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2" t="s">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="1">
         <v>0.531983739837398</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88" s="1">
         <v>0.469879518072289</v>
       </c>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2" t="s">
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J88" s="1">
         <v>0.72516533305119901</v>
       </c>
-      <c r="K88" s="2">
+      <c r="K88" s="1">
         <v>0.68763453475204706</v>
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1">
         <v>100</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89" s="1">
         <v>0.63195121951219502</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89" s="1">
         <v>0.43975903614457801</v>
       </c>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2">
+      <c r="G89" s="1"/>
+      <c r="H89" s="1">
         <v>100</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J89" s="2">
+      <c r="J89" s="1">
         <v>0.33872362199169798</v>
       </c>
-      <c r="K89" s="2">
+      <c r="K89" s="1">
         <v>0.60560276669761104</v>
       </c>
     </row>
     <row r="90" spans="1:11">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2" t="s">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="1">
         <v>0.66473170731707298</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90" s="1">
         <v>0.73795180722891496</v>
       </c>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2" t="s">
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J90" s="2">
+      <c r="J90" s="1">
         <v>0.531902780699408</v>
       </c>
-      <c r="K90" s="2">
+      <c r="K90" s="1">
         <v>0.77025800067331096</v>
       </c>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="2">
+      <c r="A91" s="1">
         <v>0.8</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>1</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="1">
         <v>0.577309018326982</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91" s="1">
         <v>0.48795180722891501</v>
       </c>
-      <c r="G91" s="2">
+      <c r="G91" s="1">
         <v>0.8</v>
       </c>
-      <c r="H91" s="2">
+      <c r="H91" s="1">
         <v>1</v>
       </c>
-      <c r="I91" s="2" t="s">
+      <c r="I91" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J91" s="2">
+      <c r="J91" s="1">
         <v>0.43272628746974701</v>
       </c>
-      <c r="K91" s="2">
+      <c r="K91" s="1">
         <v>0.67995592916020497</v>
       </c>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2" t="s">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="1">
         <v>0.621928869533659</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92" s="1">
         <v>0.71084337349397497</v>
       </c>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2" t="s">
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J92" s="2">
+      <c r="J92" s="1">
         <v>0.67497454219164299</v>
       </c>
-      <c r="K92" s="2">
+      <c r="K92" s="1">
         <v>0.57428792948665597</v>
       </c>
     </row>
     <row r="93" spans="1:11">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1">
         <v>100</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="1">
         <v>0.75307566684812199</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93" s="1">
         <v>0.40361445783132499</v>
       </c>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2">
+      <c r="G93" s="1"/>
+      <c r="H93" s="1">
         <v>100</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="I93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J93" s="2">
+      <c r="J93" s="1">
         <v>0.67688925843791703</v>
       </c>
-      <c r="K93" s="2">
+      <c r="K93" s="1">
         <v>0.53448135150575304</v>
       </c>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2" t="s">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94" s="1">
         <v>0.64184358555615995</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94" s="1">
         <v>0.52409638554216798</v>
       </c>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2" t="s">
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J94" s="2">
+      <c r="J94" s="1">
         <v>0.59867321063393297</v>
       </c>
-      <c r="K94" s="2">
+      <c r="K94" s="1">
         <v>0.87423488125356996</v>
       </c>
     </row>

</xml_diff>